<commit_message>
data: update finished formula
</commit_message>
<xml_diff>
--- a/spec/8.0对内版报告计算公式-修改2稿-20180921.xlsx
+++ b/spec/8.0对内版报告计算公式-修改2稿-20180921.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zql\0718 数据分析相关资料\0920 8.0报告计算公式-修改稿\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DADE6F-73E6-4B9E-93D8-15C2D0B2C2A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="就业与培养质量" sheetId="1" r:id="rId1"/>
@@ -21,17 +15,22 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'附表1-能力水平题目（对应能力重要性题目选项）'!$B$4:$I$72</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">就业与培养质量!$A$1:$I$118</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{BFE728B4-6D50-44E4-A18A-14ECCFA0D8F4}">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{425B22BB-1664-49DE-A230-8003E3AF65A2}">
+    <comment ref="B7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,6 +64,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Administrator:</t>
@@ -74,6 +74,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -81,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{D98E9FD4-3C5F-47A8-9989-92B87C996CE8}">
+    <comment ref="B8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,6 +90,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Administrator:</t>
@@ -98,6 +100,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -105,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{5C1224D7-70B5-49E4-AAAD-42BE7D2912C3}">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{416344C5-12DA-4079-AA32-F11801D5FF30}">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -157,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{D7308BEB-174B-4E91-B8E1-025002E1C8A8}">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -183,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{96FECB01-4AA0-4C09-AB05-E4761A10A6A9}">
+    <comment ref="B30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B31" authorId="0" shapeId="0" xr:uid="{EC6EFC5E-79D8-40D9-AE53-01F422DCE973}">
+    <comment ref="B31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -235,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{5DB724E6-2885-4279-B35F-17B01EED57BA}">
+    <comment ref="B32" authorId="0">
       <text>
         <r>
           <rPr>
@@ -261,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B78" authorId="0" shapeId="0" xr:uid="{399D5697-BA4D-4374-8774-AA3EB1301EFF}">
+    <comment ref="B78" authorId="0">
       <text>
         <r>
           <rPr>
@@ -287,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B79" authorId="0" shapeId="0" xr:uid="{21F698DC-3362-4DD6-A108-540398CB31DB}">
+    <comment ref="B79" authorId="0">
       <text>
         <r>
           <rPr>
@@ -313,7 +316,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B80" authorId="0" shapeId="0" xr:uid="{E1E91B16-E556-4B70-B96C-E32B330B4116}">
+    <comment ref="B80" authorId="0">
       <text>
         <r>
           <rPr>
@@ -339,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B81" authorId="0" shapeId="0" xr:uid="{1008DA46-6199-44DE-8C05-E11818CC05AA}">
+    <comment ref="B81" authorId="0">
       <text>
         <r>
           <rPr>
@@ -365,7 +368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="0" shapeId="0" xr:uid="{6CE1215D-E702-45AA-A7B1-CD19F31D1EBB}">
+    <comment ref="B82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -391,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0" shapeId="0" xr:uid="{82CA8465-7912-47E1-8886-9C7FFD95C3A4}">
+    <comment ref="B83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -417,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0" shapeId="0" xr:uid="{2E943431-7215-421A-A908-5B19A543B80A}">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -443,7 +446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="0" shapeId="0" xr:uid="{59C04C69-80BC-47F9-BFF2-0E8A2F748220}">
+    <comment ref="B85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -469,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B89" authorId="0" shapeId="0" xr:uid="{795F4981-0C2C-4668-88F1-62B13EA19044}">
+    <comment ref="B89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -495,7 +498,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B90" authorId="0" shapeId="0" xr:uid="{46886E33-A570-480F-92B6-7EBB8D77C6C0}">
+    <comment ref="B90" authorId="0">
       <text>
         <r>
           <rPr>
@@ -521,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0" shapeId="0" xr:uid="{5D4384DD-4BD6-4D2D-B584-9D39B85A73D8}">
+    <comment ref="B91" authorId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B92" authorId="0" shapeId="0" xr:uid="{FBF7E233-8F95-4120-B332-E8AB99644BC6}">
+    <comment ref="B92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -573,7 +576,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B99" authorId="0" shapeId="0" xr:uid="{8A02CBBF-8285-4E9F-A5E9-BD4FBECE3352}">
+    <comment ref="B99" authorId="0">
       <text>
         <r>
           <rPr>
@@ -599,7 +602,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B100" authorId="0" shapeId="0" xr:uid="{F18CDDC8-E0C8-4016-A3C3-9021865C1283}">
+    <comment ref="B100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -625,7 +628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B101" authorId="0" shapeId="0" xr:uid="{93924ED5-5365-4D86-99DE-AB71470D4C7D}">
+    <comment ref="B101" authorId="0">
       <text>
         <r>
           <rPr>
@@ -651,7 +654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B102" authorId="0" shapeId="0" xr:uid="{E5C7D198-A778-49BD-9551-B974D55005CB}">
+    <comment ref="B102" authorId="0">
       <text>
         <r>
           <rPr>
@@ -677,7 +680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0" shapeId="0" xr:uid="{4D685C18-668D-4FCF-9FEE-3318BADAAE57}">
+    <comment ref="B103" authorId="0">
       <text>
         <r>
           <rPr>
@@ -703,7 +706,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0" shapeId="0" xr:uid="{260328BB-1D7C-4735-B126-5D9EE9743DC3}">
+    <comment ref="B104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -729,7 +732,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B105" authorId="0" shapeId="0" xr:uid="{7DFD7104-AA84-48D0-87F9-63E1B11F41D4}">
+    <comment ref="B105" authorId="0">
       <text>
         <r>
           <rPr>
@@ -755,7 +758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D134" authorId="0" shapeId="0" xr:uid="{BE8FF38C-F563-444B-9042-EBE632CF186C}">
+    <comment ref="D134" authorId="0">
       <text>
         <r>
           <rPr>
@@ -781,7 +784,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D135" authorId="0" shapeId="0" xr:uid="{5C1D327F-6A2C-43DD-9153-5B8882C8C44D}">
+    <comment ref="D135" authorId="0">
       <text>
         <r>
           <rPr>
@@ -807,7 +810,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D138" authorId="0" shapeId="0" xr:uid="{D895E075-EA20-444C-B97F-CC416C54E738}">
+    <comment ref="D138" authorId="0">
       <text>
         <r>
           <rPr>
@@ -833,7 +836,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D142" authorId="0" shapeId="0" xr:uid="{AE93BC6B-6612-4A78-B90B-426B51562522}">
+    <comment ref="D142" authorId="0">
       <text>
         <r>
           <rPr>
@@ -859,7 +862,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D157" authorId="0" shapeId="0" xr:uid="{EA5105E4-2557-401A-A266-B5A7F199605A}">
+    <comment ref="D157" authorId="0">
       <text>
         <r>
           <rPr>
@@ -885,7 +888,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D158" authorId="0" shapeId="0" xr:uid="{ACCB90F4-1931-49F7-BC55-4F02199F9BFE}">
+    <comment ref="D158" authorId="0">
       <text>
         <r>
           <rPr>
@@ -4243,8 +4246,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4421,19 +4424,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -4466,7 +4456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4494,6 +4484,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4612,7 +4608,7 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -4794,58 +4790,58 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4854,22 +4850,34 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4884,26 +4892,17 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4913,9 +4912,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4927,11 +4923,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="常规_Sheet2" xfId="2" xr:uid="{1098D4A2-0130-451D-849F-B5C0B0AAF47F}"/>
+    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="常规_Sheet2" xfId="2"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -4982,7 +4993,7 @@
         <xdr:cNvPr id="4" name="图片 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5032,7 +5043,7 @@
         <xdr:cNvPr id="5" name="图片 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5080,7 +5091,7 @@
         <xdr:cNvPr id="6" name="图片 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5128,7 +5139,7 @@
         <xdr:cNvPr id="7" name="图片 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5176,7 +5187,7 @@
         <xdr:cNvPr id="8" name="图片 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5224,7 +5235,7 @@
         <xdr:cNvPr id="9" name="图片 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5272,7 +5283,7 @@
         <xdr:cNvPr id="10" name="图片 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5320,7 +5331,7 @@
         <xdr:cNvPr id="11" name="图片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5368,7 +5379,7 @@
         <xdr:cNvPr id="12" name="图片 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5416,7 +5427,7 @@
         <xdr:cNvPr id="13" name="图片 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5464,7 +5475,7 @@
         <xdr:cNvPr id="14" name="图片 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5506,7 +5517,7 @@
         <xdr:cNvPr id="15" name="图片 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5548,7 +5559,7 @@
         <xdr:cNvPr id="16" name="图片 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5590,7 +5601,7 @@
         <xdr:cNvPr id="3" name="图片 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5767E20A-F5EB-4DD4-9833-585FB89663B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5767E20A-F5EB-4DD4-9833-585FB89663B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5640,7 +5651,7 @@
         <xdr:cNvPr id="18" name="图片 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0EEEF16-CAA8-43AB-A316-BD95969A71F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0EEEF16-CAA8-43AB-A316-BD95969A71F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5690,7 +5701,7 @@
         <xdr:cNvPr id="20" name="图片 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A94936C7-3FCE-4918-B291-42F0E98CBA7D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A94936C7-3FCE-4918-B291-42F0E98CBA7D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5768,7 +5779,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5820,7 +5831,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6045,45 +6056,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.375" style="73" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.875" style="86" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.875" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.75" style="48" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="73" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.375" style="48" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.875" style="48" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.33203125" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" style="48" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.75" style="73" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" style="73" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="64"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="63" customFormat="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="89" t="s">
         <v>734</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="89" t="s">
         <v>735</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="89" t="s">
         <v>576</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="89" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="62" t="s">
@@ -6096,20 +6107,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="115.5">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
+    <row r="2" spans="1:9" ht="120">
+      <c r="A2" s="90"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
       <c r="G2" s="62" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="62"/>
       <c r="I2" s="62"/>
     </row>
-    <row r="3" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="3" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A3" s="65" t="s">
         <v>9</v>
       </c>
@@ -6132,7 +6143,7 @@
       <c r="H3" s="10"/>
       <c r="I3" s="67"/>
     </row>
-    <row r="4" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="4" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A4" s="65" t="s">
         <v>9</v>
       </c>
@@ -6157,7 +6168,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="67"/>
     </row>
-    <row r="5" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="5" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A5" s="65" t="s">
         <v>9</v>
       </c>
@@ -6182,7 +6193,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="67"/>
     </row>
-    <row r="6" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="6" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A6" s="65" t="s">
         <v>9</v>
       </c>
@@ -6207,7 +6218,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="67"/>
     </row>
-    <row r="7" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="7" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A7" s="65" t="s">
         <v>9</v>
       </c>
@@ -6232,7 +6243,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="67"/>
     </row>
-    <row r="8" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="8" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A8" s="65" t="s">
         <v>9</v>
       </c>
@@ -6257,7 +6268,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="67"/>
     </row>
-    <row r="9" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="9" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A9" s="65" t="s">
         <v>9</v>
       </c>
@@ -6324,7 +6335,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="67"/>
     </row>
-    <row r="12" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="12" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A12" s="65" t="s">
         <v>9</v>
       </c>
@@ -6349,7 +6360,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="67"/>
     </row>
-    <row r="13" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="13" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A13" s="65" t="s">
         <v>9</v>
       </c>
@@ -6374,7 +6385,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="67"/>
     </row>
-    <row r="14" spans="1:9" ht="49.5">
+    <row r="14" spans="1:9" ht="45">
       <c r="A14" s="65" t="s">
         <v>38</v>
       </c>
@@ -6395,7 +6406,7 @@
       </c>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:9" ht="49.5">
+    <row r="15" spans="1:9" ht="45">
       <c r="A15" s="65" t="s">
         <v>38</v>
       </c>
@@ -6419,7 +6430,7 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="49.5">
+    <row r="16" spans="1:9" ht="45">
       <c r="A16" s="65" t="s">
         <v>38</v>
       </c>
@@ -6443,7 +6454,7 @@
       </c>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="82.5">
+    <row r="17" spans="1:8" ht="75">
       <c r="A17" s="65" t="s">
         <v>38</v>
       </c>
@@ -6463,7 +6474,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="82.5">
+    <row r="18" spans="1:8" ht="75">
       <c r="A18" s="65" t="s">
         <v>38</v>
       </c>
@@ -6486,7 +6497,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="99">
+    <row r="19" spans="1:8" ht="90">
       <c r="A19" s="65" t="s">
         <v>38</v>
       </c>
@@ -6509,7 +6520,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="82.5">
+    <row r="20" spans="1:8" ht="75">
       <c r="A20" s="65" t="s">
         <v>38</v>
       </c>
@@ -6532,7 +6543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="115.5">
+    <row r="21" spans="1:8" ht="105">
       <c r="A21" s="65" t="s">
         <v>38</v>
       </c>
@@ -6552,7 +6563,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="115.5">
+    <row r="22" spans="1:8" ht="105">
       <c r="A22" s="65" t="s">
         <v>38</v>
       </c>
@@ -6575,7 +6586,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="115.5">
+    <row r="23" spans="1:8" ht="105">
       <c r="A23" s="65" t="s">
         <v>38</v>
       </c>
@@ -6598,7 +6609,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="99">
+    <row r="24" spans="1:8" ht="105">
       <c r="A24" s="65" t="s">
         <v>38</v>
       </c>
@@ -6618,7 +6629,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="66">
+    <row r="25" spans="1:8" ht="75">
       <c r="A25" s="65" t="s">
         <v>38</v>
       </c>
@@ -6641,7 +6652,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="66">
+    <row r="26" spans="1:8" ht="75">
       <c r="A26" s="65" t="s">
         <v>38</v>
       </c>
@@ -6664,7 +6675,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="66">
+    <row r="27" spans="1:8" ht="75">
       <c r="A27" s="65" t="s">
         <v>38</v>
       </c>
@@ -6685,7 +6696,7 @@
       </c>
       <c r="G27" s="56"/>
     </row>
-    <row r="28" spans="1:8" ht="66">
+    <row r="28" spans="1:8" ht="75">
       <c r="A28" s="65" t="s">
         <v>38</v>
       </c>
@@ -6708,7 +6719,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="66">
+    <row r="29" spans="1:8" ht="75">
       <c r="A29" s="65" t="s">
         <v>38</v>
       </c>
@@ -6731,7 +6742,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="49.5">
+    <row r="30" spans="1:8" ht="45">
       <c r="A30" s="65" t="s">
         <v>38</v>
       </c>
@@ -6752,7 +6763,7 @@
       </c>
       <c r="H30" s="23"/>
     </row>
-    <row r="31" spans="1:8" ht="49.5">
+    <row r="31" spans="1:8" ht="45">
       <c r="A31" s="65" t="s">
         <v>38</v>
       </c>
@@ -6775,7 +6786,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="49.5">
+    <row r="32" spans="1:8" ht="45">
       <c r="A32" s="65" t="s">
         <v>38</v>
       </c>
@@ -6798,7 +6809,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="66">
+    <row r="33" spans="1:9" ht="60">
       <c r="A33" s="65" t="s">
         <v>38</v>
       </c>
@@ -6821,7 +6832,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="34" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A34" s="75" t="s">
         <v>81</v>
       </c>
@@ -6846,7 +6857,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="67"/>
     </row>
-    <row r="35" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="35" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A35" s="75" t="s">
         <v>81</v>
       </c>
@@ -6871,7 +6882,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="67"/>
     </row>
-    <row r="36" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="36" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A36" s="75" t="s">
         <v>81</v>
       </c>
@@ -6896,7 +6907,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="67"/>
     </row>
-    <row r="37" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="37" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A37" s="75" t="s">
         <v>81</v>
       </c>
@@ -6921,7 +6932,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="67"/>
     </row>
-    <row r="38" spans="1:9" s="68" customFormat="1" ht="82.5">
+    <row r="38" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A38" s="75" t="s">
         <v>81</v>
       </c>
@@ -6944,7 +6955,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="67"/>
     </row>
-    <row r="39" spans="1:9" s="68" customFormat="1" ht="132">
+    <row r="39" spans="1:9" s="68" customFormat="1" ht="120">
       <c r="A39" s="75" t="s">
         <v>81</v>
       </c>
@@ -6967,7 +6978,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="67"/>
     </row>
-    <row r="40" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="40" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A40" s="75" t="s">
         <v>81</v>
       </c>
@@ -6994,7 +7005,7 @@
       </c>
       <c r="I40" s="67"/>
     </row>
-    <row r="41" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="41" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A41" s="75" t="s">
         <v>81</v>
       </c>
@@ -7021,7 +7032,7 @@
       </c>
       <c r="I41" s="67"/>
     </row>
-    <row r="42" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="42" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A42" s="75" t="s">
         <v>81</v>
       </c>
@@ -7046,7 +7057,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="67"/>
     </row>
-    <row r="43" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="43" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A43" s="75" t="s">
         <v>81</v>
       </c>
@@ -7071,7 +7082,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="67"/>
     </row>
-    <row r="44" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="44" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A44" s="75" t="s">
         <v>81</v>
       </c>
@@ -7096,7 +7107,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="67"/>
     </row>
-    <row r="45" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="45" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A45" s="75" t="s">
         <v>81</v>
       </c>
@@ -7121,7 +7132,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="67"/>
     </row>
-    <row r="46" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="46" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A46" s="75" t="s">
         <v>81</v>
       </c>
@@ -7146,7 +7157,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="67"/>
     </row>
-    <row r="47" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="47" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A47" s="75" t="s">
         <v>81</v>
       </c>
@@ -7171,7 +7182,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="67"/>
     </row>
-    <row r="48" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="48" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A48" s="75" t="s">
         <v>81</v>
       </c>
@@ -7196,7 +7207,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="67"/>
     </row>
-    <row r="49" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="49" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A49" s="75" t="s">
         <v>81</v>
       </c>
@@ -7221,7 +7232,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="67"/>
     </row>
-    <row r="50" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="50" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A50" s="75" t="s">
         <v>81</v>
       </c>
@@ -7246,7 +7257,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="67"/>
     </row>
-    <row r="51" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="51" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A51" s="75" t="s">
         <v>81</v>
       </c>
@@ -7271,7 +7282,7 @@
       <c r="H51" s="10"/>
       <c r="I51" s="67"/>
     </row>
-    <row r="52" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="52" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A52" s="75" t="s">
         <v>81</v>
       </c>
@@ -7296,7 +7307,7 @@
       <c r="H52" s="10"/>
       <c r="I52" s="67"/>
     </row>
-    <row r="53" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="53" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A53" s="75" t="s">
         <v>81</v>
       </c>
@@ -7321,7 +7332,7 @@
       <c r="H53" s="10"/>
       <c r="I53" s="67"/>
     </row>
-    <row r="54" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="54" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A54" s="75" t="s">
         <v>81</v>
       </c>
@@ -7346,7 +7357,7 @@
       <c r="H54" s="10"/>
       <c r="I54" s="67"/>
     </row>
-    <row r="55" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="55" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A55" s="75" t="s">
         <v>81</v>
       </c>
@@ -7371,7 +7382,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="67"/>
     </row>
-    <row r="56" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="56" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A56" s="75" t="s">
         <v>81</v>
       </c>
@@ -7396,7 +7407,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="67"/>
     </row>
-    <row r="57" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="57" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A57" s="75" t="s">
         <v>81</v>
       </c>
@@ -7419,7 +7430,7 @@
       <c r="H57" s="10"/>
       <c r="I57" s="67"/>
     </row>
-    <row r="58" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="58" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A58" s="75" t="s">
         <v>81</v>
       </c>
@@ -7444,7 +7455,7 @@
       <c r="H58" s="10"/>
       <c r="I58" s="67"/>
     </row>
-    <row r="59" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="59" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A59" s="75" t="s">
         <v>81</v>
       </c>
@@ -7469,7 +7480,7 @@
       <c r="H59" s="10"/>
       <c r="I59" s="67"/>
     </row>
-    <row r="60" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="60" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A60" s="75" t="s">
         <v>81</v>
       </c>
@@ -7494,7 +7505,7 @@
       <c r="H60" s="10"/>
       <c r="I60" s="67"/>
     </row>
-    <row r="61" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="61" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A61" s="75" t="s">
         <v>81</v>
       </c>
@@ -7519,7 +7530,7 @@
       <c r="H61" s="10"/>
       <c r="I61" s="67"/>
     </row>
-    <row r="62" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="62" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A62" s="75" t="s">
         <v>81</v>
       </c>
@@ -7544,7 +7555,7 @@
       <c r="H62" s="10"/>
       <c r="I62" s="67"/>
     </row>
-    <row r="63" spans="1:9" ht="33">
+    <row r="63" spans="1:9" ht="30">
       <c r="A63" s="72" t="s">
         <v>130</v>
       </c>
@@ -7564,7 +7575,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="33">
+    <row r="64" spans="1:9" ht="30">
       <c r="A64" s="72" t="s">
         <v>130</v>
       </c>
@@ -7587,7 +7598,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="33">
+    <row r="65" spans="1:9" ht="30">
       <c r="A65" s="72" t="s">
         <v>130</v>
       </c>
@@ -7607,7 +7618,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="66" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="66" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A66" s="70" t="s">
         <v>130</v>
       </c>
@@ -7630,7 +7641,7 @@
       <c r="H66" s="10"/>
       <c r="I66" s="67"/>
     </row>
-    <row r="67" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="67" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A67" s="70" t="s">
         <v>130</v>
       </c>
@@ -7655,7 +7666,7 @@
       <c r="H67" s="10"/>
       <c r="I67" s="67"/>
     </row>
-    <row r="68" spans="1:9" ht="49.5">
+    <row r="68" spans="1:9" ht="45">
       <c r="A68" s="72" t="s">
         <v>139</v>
       </c>
@@ -7676,7 +7687,7 @@
       </c>
       <c r="H68" s="10"/>
     </row>
-    <row r="69" spans="1:9" ht="66">
+    <row r="69" spans="1:9" ht="60">
       <c r="A69" s="72" t="s">
         <v>139</v>
       </c>
@@ -7696,7 +7707,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="70" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A70" s="70" t="s">
         <v>139</v>
       </c>
@@ -7719,7 +7730,7 @@
       <c r="H70" s="10"/>
       <c r="I70" s="67"/>
     </row>
-    <row r="71" spans="1:9" ht="99">
+    <row r="71" spans="1:9" ht="90">
       <c r="A71" s="72" t="s">
         <v>139</v>
       </c>
@@ -7742,7 +7753,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="72" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A72" s="72" t="s">
         <v>149</v>
       </c>
@@ -7765,7 +7776,7 @@
       <c r="H72" s="10"/>
       <c r="I72" s="67"/>
     </row>
-    <row r="73" spans="1:9" ht="49.5">
+    <row r="73" spans="1:9" ht="45">
       <c r="A73" s="72" t="s">
         <v>149</v>
       </c>
@@ -7788,7 +7799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="49.5">
+    <row r="74" spans="1:9" ht="45">
       <c r="A74" s="72" t="s">
         <v>149</v>
       </c>
@@ -7811,7 +7822,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="68" customFormat="1" ht="49.5">
+    <row r="75" spans="1:9" s="68" customFormat="1" ht="45">
       <c r="A75" s="70" t="s">
         <v>149</v>
       </c>
@@ -7834,7 +7845,7 @@
       <c r="H75" s="10"/>
       <c r="I75" s="67"/>
     </row>
-    <row r="76" spans="1:9" ht="49.5">
+    <row r="76" spans="1:9" ht="45">
       <c r="A76" s="72" t="s">
         <v>149</v>
       </c>
@@ -7858,30 +7869,32 @@
       </c>
       <c r="H76" s="10"/>
     </row>
-    <row r="77" spans="1:9" ht="66">
-      <c r="A77" s="72" t="s">
+    <row r="77" spans="1:9" s="112" customFormat="1" ht="60">
+      <c r="A77" s="108" t="s">
         <v>149</v>
       </c>
-      <c r="B77" s="72" t="s">
+      <c r="B77" s="108" t="s">
         <v>149</v>
       </c>
-      <c r="C77" s="48" t="s">
+      <c r="C77" s="109" t="s">
         <v>573</v>
       </c>
-      <c r="D77" s="48" t="s">
+      <c r="D77" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="E77" s="48" t="s">
+      <c r="E77" s="109" t="s">
         <v>159</v>
       </c>
-      <c r="F77" s="53" t="s">
+      <c r="F77" s="110" t="s">
         <v>153</v>
       </c>
-      <c r="G77" s="48" t="s">
+      <c r="G77" s="109" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" s="68" customFormat="1" ht="148.5">
+      <c r="H77" s="109"/>
+      <c r="I77" s="111"/>
+    </row>
+    <row r="78" spans="1:9" s="68" customFormat="1" ht="135">
       <c r="A78" s="75" t="s">
         <v>160</v>
       </c>
@@ -7904,7 +7917,7 @@
       <c r="H78" s="10"/>
       <c r="I78" s="67"/>
     </row>
-    <row r="79" spans="1:9" s="79" customFormat="1" ht="148.5">
+    <row r="79" spans="1:9" s="79" customFormat="1" ht="135">
       <c r="A79" s="77" t="s">
         <v>160</v>
       </c>
@@ -7929,7 +7942,7 @@
       <c r="H79" s="21"/>
       <c r="I79" s="78"/>
     </row>
-    <row r="80" spans="1:9" s="79" customFormat="1" ht="148.5">
+    <row r="80" spans="1:9" s="79" customFormat="1" ht="135">
       <c r="A80" s="77" t="s">
         <v>160</v>
       </c>
@@ -7954,7 +7967,7 @@
       <c r="H80" s="21"/>
       <c r="I80" s="78"/>
     </row>
-    <row r="81" spans="1:49" ht="66">
+    <row r="81" spans="1:49" ht="60">
       <c r="A81" s="77" t="s">
         <v>160</v>
       </c>
@@ -7977,7 +7990,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="82" spans="1:49" ht="66">
+    <row r="82" spans="1:49" ht="60">
       <c r="A82" s="77" t="s">
         <v>160</v>
       </c>
@@ -8000,7 +8013,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="83" spans="1:49" ht="66">
+    <row r="83" spans="1:49" ht="75">
       <c r="A83" s="77" t="s">
         <v>160</v>
       </c>
@@ -8022,7 +8035,7 @@
       <c r="G83" s="54"/>
       <c r="H83" s="54"/>
     </row>
-    <row r="84" spans="1:49" ht="66">
+    <row r="84" spans="1:49" ht="75">
       <c r="A84" s="77" t="s">
         <v>160</v>
       </c>
@@ -8045,7 +8058,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="85" spans="1:49" ht="66">
+    <row r="85" spans="1:49" ht="75">
       <c r="A85" s="77" t="s">
         <v>160</v>
       </c>
@@ -8068,7 +8081,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="86" spans="1:49" s="68" customFormat="1" ht="132">
+    <row r="86" spans="1:49" s="68" customFormat="1" ht="120">
       <c r="A86" s="75" t="s">
         <v>160</v>
       </c>
@@ -8091,7 +8104,7 @@
       <c r="H86" s="10"/>
       <c r="I86" s="67"/>
     </row>
-    <row r="87" spans="1:49" s="68" customFormat="1" ht="132">
+    <row r="87" spans="1:49" s="68" customFormat="1" ht="120">
       <c r="A87" s="75" t="s">
         <v>160</v>
       </c>
@@ -8156,7 +8169,7 @@
       <c r="AV87" s="80"/>
       <c r="AW87" s="80"/>
     </row>
-    <row r="88" spans="1:49" s="68" customFormat="1" ht="132">
+    <row r="88" spans="1:49" s="68" customFormat="1" ht="120">
       <c r="A88" s="75" t="s">
         <v>160</v>
       </c>
@@ -8181,7 +8194,7 @@
       <c r="H88" s="10"/>
       <c r="I88" s="67"/>
     </row>
-    <row r="89" spans="1:49" s="68" customFormat="1" ht="82.5">
+    <row r="89" spans="1:49" s="68" customFormat="1" ht="75">
       <c r="A89" s="75" t="s">
         <v>175</v>
       </c>
@@ -8242,7 +8255,7 @@
       <c r="AV89" s="80"/>
       <c r="AW89" s="80"/>
     </row>
-    <row r="90" spans="1:49" s="68" customFormat="1" ht="82.5">
+    <row r="90" spans="1:49" s="68" customFormat="1" ht="75">
       <c r="A90" s="75" t="s">
         <v>175</v>
       </c>
@@ -8303,7 +8316,7 @@
       <c r="AV90" s="80"/>
       <c r="AW90" s="80"/>
     </row>
-    <row r="91" spans="1:49" s="68" customFormat="1" ht="33">
+    <row r="91" spans="1:49" s="68" customFormat="1" ht="30">
       <c r="A91" s="75" t="s">
         <v>175</v>
       </c>
@@ -8366,7 +8379,7 @@
       <c r="AV91" s="80"/>
       <c r="AW91" s="80"/>
     </row>
-    <row r="92" spans="1:49" s="68" customFormat="1" ht="49.5">
+    <row r="92" spans="1:49" s="68" customFormat="1" ht="45">
       <c r="A92" s="75" t="s">
         <v>175</v>
       </c>
@@ -8427,7 +8440,7 @@
       <c r="AV92" s="80"/>
       <c r="AW92" s="80"/>
     </row>
-    <row r="93" spans="1:49" s="68" customFormat="1" ht="33">
+    <row r="93" spans="1:49" s="68" customFormat="1" ht="30">
       <c r="A93" s="81" t="s">
         <v>177</v>
       </c>
@@ -8490,7 +8503,7 @@
       <c r="AV93" s="80"/>
       <c r="AW93" s="80"/>
     </row>
-    <row r="94" spans="1:49" s="68" customFormat="1" ht="49.5">
+    <row r="94" spans="1:49" s="68" customFormat="1" ht="45">
       <c r="A94" s="81" t="s">
         <v>177</v>
       </c>
@@ -8555,7 +8568,7 @@
       <c r="AV94" s="80"/>
       <c r="AW94" s="80"/>
     </row>
-    <row r="95" spans="1:49" s="68" customFormat="1" ht="33">
+    <row r="95" spans="1:49" s="68" customFormat="1" ht="30">
       <c r="A95" s="81" t="s">
         <v>177</v>
       </c>
@@ -8580,7 +8593,7 @@
       <c r="H95" s="10"/>
       <c r="I95" s="67"/>
     </row>
-    <row r="96" spans="1:49" s="68" customFormat="1" ht="66">
+    <row r="96" spans="1:49" s="68" customFormat="1" ht="75">
       <c r="A96" s="83" t="s">
         <v>184</v>
       </c>
@@ -8605,7 +8618,7 @@
       <c r="H96" s="10"/>
       <c r="I96" s="67"/>
     </row>
-    <row r="97" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="97" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A97" s="83" t="s">
         <v>184</v>
       </c>
@@ -8630,7 +8643,7 @@
       <c r="H97" s="10"/>
       <c r="I97" s="67"/>
     </row>
-    <row r="98" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="98" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A98" s="83" t="s">
         <v>184</v>
       </c>
@@ -8655,7 +8668,7 @@
       <c r="H98" s="10"/>
       <c r="I98" s="67"/>
     </row>
-    <row r="99" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="99" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A99" s="83" t="s">
         <v>184</v>
       </c>
@@ -8680,7 +8693,7 @@
       <c r="H99" s="10"/>
       <c r="I99" s="67"/>
     </row>
-    <row r="100" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="100" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A100" s="83" t="s">
         <v>184</v>
       </c>
@@ -8705,7 +8718,7 @@
       <c r="H100" s="10"/>
       <c r="I100" s="67"/>
     </row>
-    <row r="101" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="101" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A101" s="83" t="s">
         <v>184</v>
       </c>
@@ -8730,7 +8743,7 @@
       <c r="H101" s="10"/>
       <c r="I101" s="67"/>
     </row>
-    <row r="102" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="102" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A102" s="83" t="s">
         <v>184</v>
       </c>
@@ -8755,7 +8768,7 @@
       <c r="H102" s="10"/>
       <c r="I102" s="67"/>
     </row>
-    <row r="103" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="103" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A103" s="83" t="s">
         <v>184</v>
       </c>
@@ -8780,7 +8793,7 @@
       <c r="H103" s="10"/>
       <c r="I103" s="67"/>
     </row>
-    <row r="104" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="104" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A104" s="83" t="s">
         <v>184</v>
       </c>
@@ -8805,7 +8818,7 @@
       <c r="H104" s="10"/>
       <c r="I104" s="67"/>
     </row>
-    <row r="105" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="105" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A105" s="83" t="s">
         <v>184</v>
       </c>
@@ -8830,7 +8843,7 @@
       <c r="H105" s="10"/>
       <c r="I105" s="67"/>
     </row>
-    <row r="106" spans="1:9" s="80" customFormat="1" ht="66">
+    <row r="106" spans="1:9" s="80" customFormat="1" ht="75">
       <c r="A106" s="83" t="s">
         <v>184</v>
       </c>
@@ -8855,7 +8868,7 @@
       <c r="H106" s="10"/>
       <c r="I106" s="67"/>
     </row>
-    <row r="107" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="107" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A107" s="83" t="s">
         <v>184</v>
       </c>
@@ -8880,7 +8893,7 @@
       <c r="H107" s="10"/>
       <c r="I107" s="67"/>
     </row>
-    <row r="108" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="108" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A108" s="83" t="s">
         <v>184</v>
       </c>
@@ -8903,7 +8916,7 @@
       <c r="H108" s="10"/>
       <c r="I108" s="67"/>
     </row>
-    <row r="109" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="109" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A109" s="83" t="s">
         <v>184</v>
       </c>
@@ -8928,7 +8941,7 @@
       <c r="H109" s="10"/>
       <c r="I109" s="67"/>
     </row>
-    <row r="110" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="110" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A110" s="83" t="s">
         <v>184</v>
       </c>
@@ -8953,7 +8966,7 @@
       <c r="H110" s="10"/>
       <c r="I110" s="67"/>
     </row>
-    <row r="111" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="111" spans="1:9" s="68" customFormat="1" ht="75">
       <c r="A111" s="83" t="s">
         <v>184</v>
       </c>
@@ -8978,7 +8991,7 @@
       <c r="H111" s="10"/>
       <c r="I111" s="67"/>
     </row>
-    <row r="112" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="112" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A112" s="83" t="s">
         <v>184</v>
       </c>
@@ -9001,7 +9014,7 @@
       <c r="H112" s="10"/>
       <c r="I112" s="67"/>
     </row>
-    <row r="113" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="113" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A113" s="75" t="s">
         <v>531</v>
       </c>
@@ -9022,7 +9035,7 @@
       <c r="H113" s="10"/>
       <c r="I113" s="67"/>
     </row>
-    <row r="114" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="114" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A114" s="75" t="s">
         <v>531</v>
       </c>
@@ -9047,7 +9060,7 @@
       <c r="H114" s="10"/>
       <c r="I114" s="67"/>
     </row>
-    <row r="115" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="115" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A115" s="75" t="s">
         <v>531</v>
       </c>
@@ -9072,7 +9085,7 @@
       <c r="H115" s="10"/>
       <c r="I115" s="67"/>
     </row>
-    <row r="116" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="116" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A116" s="75" t="s">
         <v>199</v>
       </c>
@@ -9093,7 +9106,7 @@
       <c r="H116" s="10"/>
       <c r="I116" s="67"/>
     </row>
-    <row r="117" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="117" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A117" s="75" t="s">
         <v>199</v>
       </c>
@@ -9118,7 +9131,7 @@
       <c r="H117" s="10"/>
       <c r="I117" s="67"/>
     </row>
-    <row r="118" spans="1:9" s="68" customFormat="1" ht="33">
+    <row r="118" spans="1:9" s="68" customFormat="1" ht="30">
       <c r="A118" s="75" t="s">
         <v>199</v>
       </c>
@@ -9143,7 +9156,7 @@
       <c r="H118" s="10"/>
       <c r="I118" s="67"/>
     </row>
-    <row r="119" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="119" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A119" s="75" t="s">
         <v>306</v>
       </c>
@@ -9164,7 +9177,7 @@
       <c r="H119" s="10"/>
       <c r="I119" s="67"/>
     </row>
-    <row r="120" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="120" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A120" s="75" t="s">
         <v>306</v>
       </c>
@@ -9189,7 +9202,7 @@
       <c r="H120" s="10"/>
       <c r="I120" s="67"/>
     </row>
-    <row r="121" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="121" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A121" s="75" t="s">
         <v>306</v>
       </c>
@@ -9214,7 +9227,7 @@
       <c r="H121" s="10"/>
       <c r="I121" s="67"/>
     </row>
-    <row r="122" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="122" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A122" s="75" t="s">
         <v>306</v>
       </c>
@@ -9237,7 +9250,7 @@
       <c r="H122" s="10"/>
       <c r="I122" s="67"/>
     </row>
-    <row r="123" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="123" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A123" s="75" t="s">
         <v>306</v>
       </c>
@@ -9262,7 +9275,7 @@
       <c r="H123" s="10"/>
       <c r="I123" s="67"/>
     </row>
-    <row r="124" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="124" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A124" s="75" t="s">
         <v>306</v>
       </c>
@@ -9287,7 +9300,7 @@
       <c r="H124" s="10"/>
       <c r="I124" s="67"/>
     </row>
-    <row r="125" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="125" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A125" s="75" t="s">
         <v>306</v>
       </c>
@@ -9308,7 +9321,7 @@
       <c r="H125" s="10"/>
       <c r="I125" s="67"/>
     </row>
-    <row r="126" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="126" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A126" s="75" t="s">
         <v>306</v>
       </c>
@@ -9333,7 +9346,7 @@
       <c r="H126" s="10"/>
       <c r="I126" s="67"/>
     </row>
-    <row r="127" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="127" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A127" s="75" t="s">
         <v>306</v>
       </c>
@@ -9358,7 +9371,7 @@
       <c r="H127" s="10"/>
       <c r="I127" s="67"/>
     </row>
-    <row r="128" spans="1:9" s="68" customFormat="1" ht="66">
+    <row r="128" spans="1:9" s="68" customFormat="1" ht="60">
       <c r="A128" s="75" t="s">
         <v>306</v>
       </c>
@@ -9379,7 +9392,7 @@
       <c r="H128" s="10"/>
       <c r="I128" s="67"/>
     </row>
-    <row r="129" spans="1:50" s="68" customFormat="1" ht="66">
+    <row r="129" spans="1:50" s="68" customFormat="1" ht="60">
       <c r="A129" s="75" t="s">
         <v>306</v>
       </c>
@@ -9404,7 +9417,7 @@
       <c r="H129" s="10"/>
       <c r="I129" s="67"/>
     </row>
-    <row r="130" spans="1:50" ht="66">
+    <row r="130" spans="1:50" ht="60">
       <c r="A130" s="77" t="s">
         <v>306</v>
       </c>
@@ -9465,7 +9478,7 @@
       <c r="AW130" s="68"/>
       <c r="AX130" s="68"/>
     </row>
-    <row r="131" spans="1:50" ht="66">
+    <row r="131" spans="1:50" ht="60">
       <c r="A131" s="83" t="s">
         <v>306</v>
       </c>
@@ -9532,10 +9545,10 @@
       <c r="C132" s="23" t="s">
         <v>705</v>
       </c>
-      <c r="D132" s="89" t="s">
+      <c r="D132" s="93" t="s">
         <v>220</v>
       </c>
-      <c r="E132" s="90"/>
+      <c r="E132" s="94"/>
       <c r="F132" s="10" t="s">
         <v>221</v>
       </c>
@@ -9553,10 +9566,10 @@
       <c r="C133" s="23" t="s">
         <v>706</v>
       </c>
-      <c r="D133" s="89" t="s">
+      <c r="D133" s="93" t="s">
         <v>222</v>
       </c>
-      <c r="E133" s="90"/>
+      <c r="E133" s="94"/>
       <c r="F133" s="10" t="s">
         <v>732</v>
       </c>
@@ -9574,10 +9587,10 @@
       <c r="C134" s="23" t="s">
         <v>707</v>
       </c>
-      <c r="D134" s="91" t="s">
+      <c r="D134" s="95" t="s">
         <v>225</v>
       </c>
-      <c r="E134" s="92"/>
+      <c r="E134" s="96"/>
       <c r="F134" s="10" t="s">
         <v>226</v>
       </c>
@@ -9595,10 +9608,10 @@
       <c r="C135" s="23" t="s">
         <v>708</v>
       </c>
-      <c r="D135" s="91" t="s">
+      <c r="D135" s="95" t="s">
         <v>227</v>
       </c>
-      <c r="E135" s="92"/>
+      <c r="E135" s="96"/>
       <c r="F135" s="10" t="s">
         <v>228</v>
       </c>
@@ -9618,10 +9631,10 @@
       <c r="C136" s="23" t="s">
         <v>709</v>
       </c>
-      <c r="D136" s="89" t="s">
+      <c r="D136" s="93" t="s">
         <v>231</v>
       </c>
-      <c r="E136" s="90"/>
+      <c r="E136" s="94"/>
       <c r="F136" s="10" t="s">
         <v>221</v>
       </c>
@@ -9639,10 +9652,10 @@
       <c r="C137" s="23" t="s">
         <v>710</v>
       </c>
-      <c r="D137" s="89" t="s">
+      <c r="D137" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="E137" s="90"/>
+      <c r="E137" s="94"/>
       <c r="F137" s="10" t="s">
         <v>223</v>
       </c>
@@ -9660,10 +9673,10 @@
       <c r="C138" s="23" t="s">
         <v>711</v>
       </c>
-      <c r="D138" s="91" t="s">
+      <c r="D138" s="95" t="s">
         <v>233</v>
       </c>
-      <c r="E138" s="92"/>
+      <c r="E138" s="96"/>
       <c r="F138" s="10" t="s">
         <v>226</v>
       </c>
@@ -9681,10 +9694,10 @@
       <c r="C139" s="23" t="s">
         <v>712</v>
       </c>
-      <c r="D139" s="95" t="s">
+      <c r="D139" s="97" t="s">
         <v>234</v>
       </c>
-      <c r="E139" s="96"/>
+      <c r="E139" s="98"/>
       <c r="F139" s="10" t="s">
         <v>228</v>
       </c>
@@ -9702,10 +9715,10 @@
       <c r="C140" s="23" t="s">
         <v>713</v>
       </c>
-      <c r="D140" s="89" t="s">
+      <c r="D140" s="93" t="s">
         <v>236</v>
       </c>
-      <c r="E140" s="90"/>
+      <c r="E140" s="94"/>
       <c r="F140" s="10" t="s">
         <v>221</v>
       </c>
@@ -9723,10 +9736,10 @@
       <c r="C141" s="23" t="s">
         <v>714</v>
       </c>
-      <c r="D141" s="89" t="s">
+      <c r="D141" s="93" t="s">
         <v>237</v>
       </c>
-      <c r="E141" s="90"/>
+      <c r="E141" s="94"/>
       <c r="F141" s="10" t="s">
         <v>223</v>
       </c>
@@ -9744,10 +9757,10 @@
       <c r="C142" s="23" t="s">
         <v>715</v>
       </c>
-      <c r="D142" s="91" t="s">
+      <c r="D142" s="95" t="s">
         <v>318</v>
       </c>
-      <c r="E142" s="92"/>
+      <c r="E142" s="96"/>
       <c r="F142" s="10" t="s">
         <v>226</v>
       </c>
@@ -9765,10 +9778,10 @@
       <c r="C143" s="23" t="s">
         <v>716</v>
       </c>
-      <c r="D143" s="95" t="s">
+      <c r="D143" s="97" t="s">
         <v>238</v>
       </c>
-      <c r="E143" s="96"/>
+      <c r="E143" s="98"/>
       <c r="F143" s="10" t="s">
         <v>228</v>
       </c>
@@ -9786,10 +9799,10 @@
       <c r="C144" s="23" t="s">
         <v>717</v>
       </c>
-      <c r="D144" s="89" t="s">
+      <c r="D144" s="93" t="s">
         <v>240</v>
       </c>
-      <c r="E144" s="90"/>
+      <c r="E144" s="94"/>
       <c r="F144" s="10" t="s">
         <v>221</v>
       </c>
@@ -9807,10 +9820,10 @@
       <c r="C145" s="23" t="s">
         <v>718</v>
       </c>
-      <c r="D145" s="89" t="s">
+      <c r="D145" s="93" t="s">
         <v>241</v>
       </c>
-      <c r="E145" s="90"/>
+      <c r="E145" s="94"/>
       <c r="F145" s="10" t="s">
         <v>223</v>
       </c>
@@ -9828,10 +9841,10 @@
       <c r="C146" s="23" t="s">
         <v>719</v>
       </c>
-      <c r="D146" s="89" t="s">
+      <c r="D146" s="93" t="s">
         <v>243</v>
       </c>
-      <c r="E146" s="90"/>
+      <c r="E146" s="94"/>
       <c r="F146" s="10" t="s">
         <v>221</v>
       </c>
@@ -9849,10 +9862,10 @@
       <c r="C147" s="23" t="s">
         <v>720</v>
       </c>
-      <c r="D147" s="89" t="s">
+      <c r="D147" s="93" t="s">
         <v>244</v>
       </c>
-      <c r="E147" s="90"/>
+      <c r="E147" s="94"/>
       <c r="F147" s="10" t="s">
         <v>223</v>
       </c>
@@ -9870,10 +9883,10 @@
       <c r="C148" s="23" t="s">
         <v>721</v>
       </c>
-      <c r="D148" s="89" t="s">
+      <c r="D148" s="93" t="s">
         <v>319</v>
       </c>
-      <c r="E148" s="90"/>
+      <c r="E148" s="94"/>
       <c r="F148" s="10" t="s">
         <v>221</v>
       </c>
@@ -9891,10 +9904,10 @@
       <c r="C149" s="23" t="s">
         <v>722</v>
       </c>
-      <c r="D149" s="89" t="s">
+      <c r="D149" s="93" t="s">
         <v>733</v>
       </c>
-      <c r="E149" s="90"/>
+      <c r="E149" s="94"/>
       <c r="F149" s="10" t="s">
         <v>223</v>
       </c>
@@ -9912,10 +9925,10 @@
       <c r="C150" s="23" t="s">
         <v>723</v>
       </c>
-      <c r="D150" s="89" t="s">
+      <c r="D150" s="93" t="s">
         <v>700</v>
       </c>
-      <c r="E150" s="90"/>
+      <c r="E150" s="94"/>
       <c r="F150" s="10" t="s">
         <v>221</v>
       </c>
@@ -9933,10 +9946,10 @@
       <c r="C151" s="23" t="s">
         <v>724</v>
       </c>
-      <c r="D151" s="89" t="s">
+      <c r="D151" s="93" t="s">
         <v>701</v>
       </c>
-      <c r="E151" s="90"/>
+      <c r="E151" s="94"/>
       <c r="F151" s="10" t="s">
         <v>223</v>
       </c>
@@ -9954,10 +9967,10 @@
       <c r="C152" s="23" t="s">
         <v>725</v>
       </c>
-      <c r="D152" s="89" t="s">
+      <c r="D152" s="93" t="s">
         <v>702</v>
       </c>
-      <c r="E152" s="90"/>
+      <c r="E152" s="94"/>
       <c r="F152" s="10" t="s">
         <v>221</v>
       </c>
@@ -9975,10 +9988,10 @@
       <c r="C153" s="23" t="s">
         <v>726</v>
       </c>
-      <c r="D153" s="89" t="s">
+      <c r="D153" s="93" t="s">
         <v>703</v>
       </c>
-      <c r="E153" s="90"/>
+      <c r="E153" s="94"/>
       <c r="F153" s="10" t="s">
         <v>223</v>
       </c>
@@ -9996,10 +10009,10 @@
       <c r="C154" s="23" t="s">
         <v>727</v>
       </c>
-      <c r="D154" s="89" t="s">
+      <c r="D154" s="93" t="s">
         <v>249</v>
       </c>
-      <c r="E154" s="90"/>
+      <c r="E154" s="94"/>
       <c r="F154" s="10" t="s">
         <v>223</v>
       </c>
@@ -10017,10 +10030,10 @@
       <c r="C155" s="23" t="s">
         <v>728</v>
       </c>
-      <c r="D155" s="89" t="s">
+      <c r="D155" s="93" t="s">
         <v>251</v>
       </c>
-      <c r="E155" s="90"/>
+      <c r="E155" s="94"/>
       <c r="F155" s="10" t="s">
         <v>252</v>
       </c>
@@ -10038,10 +10051,10 @@
       <c r="C156" s="23" t="s">
         <v>729</v>
       </c>
-      <c r="D156" s="89" t="s">
+      <c r="D156" s="93" t="s">
         <v>251</v>
       </c>
-      <c r="E156" s="90"/>
+      <c r="E156" s="94"/>
       <c r="F156" s="10" t="s">
         <v>252</v>
       </c>
@@ -10059,10 +10072,10 @@
       <c r="C157" s="23" t="s">
         <v>730</v>
       </c>
-      <c r="D157" s="93" t="s">
+      <c r="D157" s="91" t="s">
         <v>320</v>
       </c>
-      <c r="E157" s="94"/>
+      <c r="E157" s="92"/>
       <c r="F157" s="10" t="s">
         <v>252</v>
       </c>
@@ -10080,10 +10093,10 @@
       <c r="C158" s="23" t="s">
         <v>731</v>
       </c>
-      <c r="D158" s="93" t="s">
+      <c r="D158" s="91" t="s">
         <v>320</v>
       </c>
-      <c r="E158" s="94"/>
+      <c r="E158" s="92"/>
       <c r="F158" s="10" t="s">
         <v>252</v>
       </c>
@@ -10139,23 +10152,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D156:E156"/>
     <mergeCell ref="D132:E132"/>
     <mergeCell ref="D133:E133"/>
     <mergeCell ref="D134:E134"/>
@@ -10172,45 +10168,67 @@
     <mergeCell ref="D143:E143"/>
     <mergeCell ref="D136:E136"/>
     <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5E9A2A-F9D1-4191-B240-0628E402F028}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I73"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="4" max="4" width="29.75" style="47" customWidth="1"/>
-    <col min="8" max="8" width="17.375" customWidth="1"/>
-    <col min="9" max="9" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="47" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="25" customFormat="1" ht="132.75" customHeight="1">
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="101" t="s">
         <v>322</v>
       </c>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
     </row>
     <row r="2" spans="2:9" s="25" customFormat="1">
       <c r="B2" s="26"/>
@@ -10242,15 +10260,15 @@
       <c r="D4" s="43" t="s">
         <v>325</v>
       </c>
-      <c r="E4" s="102" t="s">
+      <c r="E4" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-    </row>
-    <row r="5" spans="2:9" s="25" customFormat="1" ht="27">
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+    </row>
+    <row r="5" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B5" s="99" t="s">
         <v>327</v>
       </c>
@@ -10276,7 +10294,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="6" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="6" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B6" s="99"/>
       <c r="C6" s="31" t="s">
         <v>335</v>
@@ -10300,7 +10318,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="7" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B7" s="99" t="s">
         <v>337</v>
       </c>
@@ -10326,7 +10344,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="8" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="8" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B8" s="99"/>
       <c r="C8" s="32" t="s">
         <v>340</v>
@@ -10350,8 +10368,8 @@
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="2:9" s="25" customFormat="1" ht="40.5">
-      <c r="B9" s="103" t="s">
+    <row r="9" spans="2:9" s="25" customFormat="1" ht="42">
+      <c r="B9" s="100" t="s">
         <v>342</v>
       </c>
       <c r="C9" s="31" t="s">
@@ -10376,8 +10394,8 @@
         <v>334</v>
       </c>
     </row>
-    <row r="10" spans="2:9" s="25" customFormat="1" ht="27">
-      <c r="B10" s="103"/>
+    <row r="10" spans="2:9" s="25" customFormat="1" ht="28">
+      <c r="B10" s="100"/>
       <c r="C10" s="31" t="s">
         <v>345</v>
       </c>
@@ -10426,7 +10444,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="12" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B12" s="99"/>
       <c r="C12" s="31" t="s">
         <v>350</v>
@@ -10450,7 +10468,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="13" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B13" s="99" t="s">
         <v>352</v>
       </c>
@@ -10476,7 +10494,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="14" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="14" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B14" s="99"/>
       <c r="C14" s="31" t="s">
         <v>355</v>
@@ -10500,7 +10518,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="15" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="15" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B15" s="99"/>
       <c r="C15" s="31" t="s">
         <v>357</v>
@@ -10524,7 +10542,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="16" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="16" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B16" s="99"/>
       <c r="C16" s="31" t="s">
         <v>359</v>
@@ -10548,7 +10566,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="17" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="17" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B17" s="99"/>
       <c r="C17" s="31" t="s">
         <v>361</v>
@@ -10572,7 +10590,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="18" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="18" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B18" s="99" t="s">
         <v>363</v>
       </c>
@@ -10598,7 +10616,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="19" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B19" s="99"/>
       <c r="C19" s="32" t="s">
         <v>366</v>
@@ -10622,7 +10640,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="20" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="20" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B20" s="99"/>
       <c r="C20" s="31" t="s">
         <v>368</v>
@@ -10646,7 +10664,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="21" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="21" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B21" s="99"/>
       <c r="C21" s="31" t="s">
         <v>370</v>
@@ -10670,7 +10688,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="22" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="22" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B22" s="99"/>
       <c r="C22" s="31" t="s">
         <v>372</v>
@@ -10694,7 +10712,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="23" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B23" s="99" t="s">
         <v>374</v>
       </c>
@@ -10720,7 +10738,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="24" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B24" s="99"/>
       <c r="C24" s="32" t="s">
         <v>377</v>
@@ -10744,7 +10762,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="25" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="25" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B25" s="99" t="s">
         <v>379</v>
       </c>
@@ -10770,7 +10788,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="26" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="26" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B26" s="99"/>
       <c r="C26" s="32" t="s">
         <v>382</v>
@@ -10820,7 +10838,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="28" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="28" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B28" s="99"/>
       <c r="C28" s="31" t="s">
         <v>387</v>
@@ -10844,7 +10862,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="29" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="29" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B29" s="99"/>
       <c r="C29" s="31" t="s">
         <v>389</v>
@@ -10868,7 +10886,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="30" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="30" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B30" s="99" t="s">
         <v>391</v>
       </c>
@@ -10894,7 +10912,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="31" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="31" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B31" s="99"/>
       <c r="C31" s="31" t="s">
         <v>394</v>
@@ -10944,7 +10962,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="33" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="33" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B33" s="99"/>
       <c r="C33" s="31" t="s">
         <v>399</v>
@@ -10968,8 +10986,8 @@
         <v>334</v>
       </c>
     </row>
-    <row r="34" spans="2:9" s="25" customFormat="1" ht="27">
-      <c r="B34" s="103" t="s">
+    <row r="34" spans="2:9" s="25" customFormat="1" ht="28">
+      <c r="B34" s="100" t="s">
         <v>401</v>
       </c>
       <c r="C34" s="31" t="s">
@@ -10994,8 +11012,8 @@
         <v>334</v>
       </c>
     </row>
-    <row r="35" spans="2:9" s="25" customFormat="1" ht="27">
-      <c r="B35" s="103"/>
+    <row r="35" spans="2:9" s="25" customFormat="1" ht="28">
+      <c r="B35" s="100"/>
       <c r="C35" s="31" t="s">
         <v>404</v>
       </c>
@@ -11018,8 +11036,8 @@
         <v>334</v>
       </c>
     </row>
-    <row r="36" spans="2:9" s="25" customFormat="1" ht="27">
-      <c r="B36" s="103"/>
+    <row r="36" spans="2:9" s="25" customFormat="1" ht="28">
+      <c r="B36" s="100"/>
       <c r="C36" s="31" t="s">
         <v>406</v>
       </c>
@@ -11068,7 +11086,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="38" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="38" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B38" s="99"/>
       <c r="C38" s="31" t="s">
         <v>411</v>
@@ -11092,7 +11110,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="39" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="39" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B39" s="99" t="s">
         <v>413</v>
       </c>
@@ -11118,7 +11136,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="40" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="40" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B40" s="99"/>
       <c r="C40" s="31" t="s">
         <v>416</v>
@@ -11142,7 +11160,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="41" spans="2:9" s="25" customFormat="1" ht="27.75">
+    <row r="41" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B41" s="99" t="s">
         <v>418</v>
       </c>
@@ -11168,7 +11186,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="42" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="42" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B42" s="99"/>
       <c r="C42" s="31" t="s">
         <v>421</v>
@@ -11192,7 +11210,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="43" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="43" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B43" s="99"/>
       <c r="C43" s="31" t="s">
         <v>423</v>
@@ -11242,7 +11260,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="45" spans="2:9" s="38" customFormat="1" ht="27">
+    <row r="45" spans="2:9" s="38" customFormat="1" ht="28">
       <c r="B45" s="99"/>
       <c r="C45" s="37" t="s">
         <v>428</v>
@@ -11290,7 +11308,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="47" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="47" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B47" s="99"/>
       <c r="C47" s="32" t="s">
         <v>432</v>
@@ -11388,7 +11406,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="51" spans="2:9" s="38" customFormat="1" ht="27">
+    <row r="51" spans="2:9" s="38" customFormat="1" ht="28">
       <c r="B51" s="99"/>
       <c r="C51" s="37" t="s">
         <v>441</v>
@@ -11438,7 +11456,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="53" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="53" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B53" s="99"/>
       <c r="C53" s="31" t="s">
         <v>446</v>
@@ -11486,7 +11504,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="55" spans="2:9" s="38" customFormat="1" ht="27">
+    <row r="55" spans="2:9" s="38" customFormat="1" ht="28">
       <c r="B55" s="99"/>
       <c r="C55" s="37" t="s">
         <v>450</v>
@@ -11608,7 +11626,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="60" spans="2:9" s="38" customFormat="1" ht="27">
+    <row r="60" spans="2:9" s="38" customFormat="1" ht="28">
       <c r="B60" s="99"/>
       <c r="C60" s="37" t="s">
         <v>461</v>
@@ -11632,7 +11650,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="61" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="61" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B61" s="99"/>
       <c r="C61" s="31" t="s">
         <v>463</v>
@@ -11682,7 +11700,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="63" spans="2:9" s="38" customFormat="1" ht="27">
+    <row r="63" spans="2:9" s="38" customFormat="1" ht="28">
       <c r="B63" s="99"/>
       <c r="C63" s="37" t="s">
         <v>468</v>
@@ -11706,7 +11724,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="64" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="64" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B64" s="99"/>
       <c r="C64" s="31" t="s">
         <v>470</v>
@@ -11754,7 +11772,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="66" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="66" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B66" s="99"/>
       <c r="C66" s="31" t="s">
         <v>474</v>
@@ -11852,7 +11870,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="70" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="70" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B70" s="99" t="s">
         <v>483</v>
       </c>
@@ -11902,7 +11920,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="72" spans="2:9" s="25" customFormat="1" ht="27">
+    <row r="72" spans="2:9" s="25" customFormat="1" ht="28">
       <c r="B72" s="99"/>
       <c r="C72" s="32" t="s">
         <v>488</v>
@@ -11937,13 +11955,25 @@
       <c r="I73" s="29"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:I72" xr:uid="{AD37797C-D177-4FEC-B286-4E9C9C2F74B1}">
+  <autoFilter ref="B4:I72">
     <filterColumn colId="3" showButton="0"/>
     <filterColumn colId="4" showButton="0"/>
     <filterColumn colId="5" showButton="0"/>
     <filterColumn colId="6" showButton="0"/>
   </autoFilter>
   <mergeCells count="24">
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B29"/>
     <mergeCell ref="B70:B72"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B34:B36"/>
@@ -11956,42 +11986,35 @@
     <mergeCell ref="B56:B61"/>
     <mergeCell ref="B62:B67"/>
     <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B29"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="15.25" customWidth="1"/>
-    <col min="3" max="3" width="33.125" customWidth="1"/>
-    <col min="4" max="4" width="29.375" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
     <col min="5" max="5" width="22.5" customWidth="1"/>
     <col min="6" max="6" width="51.5" customWidth="1"/>
-    <col min="7" max="7" width="23.75" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27.75" customHeight="1">
@@ -12030,7 +12053,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="49.5">
+    <row r="3" spans="1:8" ht="45">
       <c r="A3" s="4" t="s">
         <v>253</v>
       </c>
@@ -12052,7 +12075,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="49.5">
+    <row r="4" spans="1:8" ht="45">
       <c r="A4" s="4" t="s">
         <v>253</v>
       </c>
@@ -12394,7 +12417,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="99">
+    <row r="19" spans="1:9" ht="90">
       <c r="A19" s="4" t="s">
         <v>253</v>
       </c>
@@ -12442,7 +12465,7 @@
       </c>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="49.5">
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="45">
       <c r="A21" s="15" t="s">
         <v>274</v>
       </c>
@@ -12577,5 +12600,10 @@
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>